<commit_message>
Updated Excel calculations of AGC input/output
</commit_message>
<xml_diff>
--- a/.mchp_private/reports/dpsk3-power-buck-agc.xlsx
+++ b/.mchp_private/reports/dpsk3-power-buck-agc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Firmware\MCU16ASMPS_CodeExamples\dpsk3-power-buck-adaptive-gain-control\.mchp_private\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49016E1D-C40C-43B7-A23B-23F113911A12}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF3495D8-E095-4B80-84F6-B606B75DE5AD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5115" yWindow="540" windowWidth="21600" windowHeight="11505" xr2:uid="{3D56D478-F40D-45D1-8FA6-0836E8ED2300}"/>
   </bookViews>
@@ -672,7 +672,7 @@
   <dimension ref="A1:L28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14:K15"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -950,6 +950,7 @@
         <f>$C$7/B7</f>
         <v>2.85</v>
       </c>
+      <c r="I8" s="12"/>
       <c r="J8" t="s">
         <v>46</v>
       </c>
@@ -1006,6 +1007,7 @@
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I10" s="12"/>
       <c r="J10" t="s">
         <v>47</v>
       </c>
@@ -1025,6 +1027,7 @@
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
       <c r="D11" s="8"/>
+      <c r="I11" s="12"/>
       <c r="J11" t="s">
         <v>24</v>
       </c>
@@ -1065,7 +1068,7 @@
         <f>"0x" &amp; DEC2HEX(G12, 4)</f>
         <v>0x08CF</v>
       </c>
-      <c r="I12" t="s">
+      <c r="I12" s="12" t="s">
         <v>40</v>
       </c>
       <c r="J12" t="s">
@@ -1076,8 +1079,8 @@
         <v>0.17543512658227847</v>
       </c>
       <c r="L12" s="12" t="str">
-        <f>"0x" &amp; DEC2HEX(K12,4)</f>
-        <v>0x0000</v>
+        <f>"0x" &amp; DEC2HEX(INT(K12*2^15),4)</f>
+        <v>0x1674</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -1108,7 +1111,7 @@
         <f t="shared" ref="H13" si="8">"0x" &amp; DEC2HEX(G13, 4)</f>
         <v>0xFFFE</v>
       </c>
-      <c r="I13" t="s">
+      <c r="I13" s="12" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1140,7 +1143,7 @@
         <f>"0x" &amp; DEC2HEX(G14, 4)</f>
         <v>0x0377</v>
       </c>
-      <c r="I14" t="s">
+      <c r="I14" s="12" t="s">
         <v>38</v>
       </c>
     </row>

</xml_diff>